<commit_message>
Improved GUI + Bug fixes
* Transposed the Diagnosis Table
* Fix ratio8_callback bug
* Updated the progress slider
* Added some tooltip strings to the  DGA_UI figure
* Put icons on the Dataset/Method add and remove buttons
* Replaced the InputMode dropdown list with a radio button for simpler
and more consistent user experience
* Added warning message when an attempt to run DGA in the dataset input
mode without selecting a dataset.
* Allowed the user to choose file name and location for exported tables
and graphs and warn before overwriting existing files.
* Increased the font for exported graph and replaced diagnosis codes
with the corresponding symbols
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="23235" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="24495" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Filename</t>
   </si>
@@ -33,6 +33,93 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Duval</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Duval.m</t>
+  </si>
+  <si>
+    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
+2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
+  </si>
+  <si>
+    <t>Rogers' 4</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Roger4.m</t>
+  </si>
+  <si>
+    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
+ 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>IEC 60599</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_IEC.m</t>
+  </si>
+  <si>
+    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
+  </si>
+  <si>
+    <t>Cond. prob.</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Cond_Prob.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_ANN.m</t>
+  </si>
+  <si>
+    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
+  </si>
+  <si>
+    <t>IEC 60599 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\IEC_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
+  </si>
+  <si>
+    <t>Rogers' 4 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\ROG_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t>.\methods\cpp\debug\DGA_Test.exe</t>
+  </si>
+  <si>
+    <t>Duval (C++)</t>
+  </si>
+  <si>
+    <t>Clustering (Fortran)</t>
+  </si>
+  <si>
+    <t>To demonstrate the integration of DAG method implementation in C++ language</t>
   </si>
   <si>
     <t>Lab Data (240)</t>
@@ -144,111 +231,12 @@
     <t>CombinedSet_(68)</t>
   </si>
   <si>
-    <t>./datasets/dataset12_(68).xls</t>
+    <t>./datasets/dataset12_(68).xlsx</t>
   </si>
   <si>
     <t>1 Rahul Soni and Kaushal R. Chaudhari “A Novel Proposed Model to Diagnose Incipient Faults of Power Transformer Using Dissolved Gas Analysis by Ratio methods”, International Conference on Computation of Power, Energy, Information and Communication, April 2015.
 2. Guanjun ZHANG, Koichi YASUOKA, Shozo ISHII “Application of Fuzzy Equivalent Matrix for Fault Diagnosis of Oil-immersed Insulation”, Proceedings of 13th International Conference on Dielectric Liquids ( ICDL ‘99 ), Nara, Japan, July 20-25, 1999.   
 3. O.E Gouda, Saber Salem and Salah Hamdy El-Hoshy “Power transformer incipient faults diagnosis based on dissolved gas analysis”, TELKOMNIKA Indonesian Journal of Electrical Engineering Vol. 17, No. 1, pp. 10 ~ 16,  January 2016.</t>
-  </si>
-  <si>
-    <t>Duval triangle method</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Duval.m</t>
-  </si>
-  <si>
-    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
-2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
-  </si>
-  <si>
-    <t>Rogers' four ratios</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Roger4.m</t>
-  </si>
-  <si>
-    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
- 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>IEC 60599</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_IEC.m</t>
-  </si>
-  <si>
-    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Key.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Clustering approach (Fortran)</t>
-  </si>
-  <si>
-    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
-  </si>
-  <si>
-    <t>Conditional Probability approach</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Cond_Prob.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
-  </si>
-  <si>
-    <t>ANN diagnosis technique</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_ANN.m</t>
-  </si>
-  <si>
-    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
-  </si>
-  <si>
-    <t>IEC 60599_Refining</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_IEC_MODIFIED.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
-  </si>
-  <si>
-    <t>Rogers' four ratios_Refining</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_ROG_MODIFIED.m</t>
-  </si>
-  <si>
-    <t>Duval With Error</t>
-  </si>
-  <si>
-    <t>.\methods\Copy_of_DGA_Duval.m</t>
-  </si>
-  <si>
-    <t>C++ Sample</t>
-  </si>
-  <si>
-    <t>.\methods\cpp\debug\DGA_Test.exe</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1185,13 +1173,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="165">
@@ -1199,13 +1187,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="165">
@@ -1213,125 +1201,97 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="135">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1344,15 +1304,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="76" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1375,13 +1335,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
@@ -1389,13 +1349,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
@@ -1403,13 +1363,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
@@ -1417,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
@@ -1431,13 +1391,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
@@ -1445,13 +1405,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
@@ -1459,13 +1419,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="255">
@@ -1473,13 +1433,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60">
@@ -1487,13 +1447,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45">
@@ -1501,13 +1461,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60">
@@ -1515,13 +1475,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="180">
@@ -1529,13 +1489,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes and GUI layout improvements
* Fix close/save bug in Datasets_Edit and Methods_Edit figures
* Improve the DGA_UI layout
* Refactor ExportViews functionality
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="24495" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="432" windowWidth="24492" windowHeight="15972"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>Filename</t>
   </si>
@@ -33,93 +33,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Duval</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Duval.m</t>
-  </si>
-  <si>
-    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
-2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
-  </si>
-  <si>
-    <t>Rogers' 4</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Roger4.m</t>
-  </si>
-  <si>
-    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
- 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>IEC 60599</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_IEC.m</t>
-  </si>
-  <si>
-    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
-  </si>
-  <si>
-    <t>Cond. prob.</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Cond_Prob.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
-  </si>
-  <si>
-    <t>ANN</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_ANN.m</t>
-  </si>
-  <si>
-    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
-  </si>
-  <si>
-    <t>IEC 60599 Refined</t>
-  </si>
-  <si>
-    <t>.\methods\IEC_REFINNING_NEW.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
-  </si>
-  <si>
-    <t>Rogers' 4 Refined</t>
-  </si>
-  <si>
-    <t>.\methods\ROG_REFINNING_NEW.m</t>
-  </si>
-  <si>
-    <t>.\methods\cpp\debug\DGA_Test.exe</t>
-  </si>
-  <si>
-    <t>Duval (C++)</t>
-  </si>
-  <si>
-    <t>Clustering (Fortran)</t>
-  </si>
-  <si>
-    <t>To demonstrate the integration of DAG method implementation in C++ language</t>
   </si>
   <si>
     <t>Lab Data (240)</t>
@@ -237,6 +150,102 @@
     <t>1 Rahul Soni and Kaushal R. Chaudhari “A Novel Proposed Model to Diagnose Incipient Faults of Power Transformer Using Dissolved Gas Analysis by Ratio methods”, International Conference on Computation of Power, Energy, Information and Communication, April 2015.
 2. Guanjun ZHANG, Koichi YASUOKA, Shozo ISHII “Application of Fuzzy Equivalent Matrix for Fault Diagnosis of Oil-immersed Insulation”, Proceedings of 13th International Conference on Dielectric Liquids ( ICDL ‘99 ), Nara, Japan, July 20-25, 1999.   
 3. O.E Gouda, Saber Salem and Salah Hamdy El-Hoshy “Power transformer incipient faults diagnosis based on dissolved gas analysis”, TELKOMNIKA Indonesian Journal of Electrical Engineering Vol. 17, No. 1, pp. 10 ~ 16,  January 2016.</t>
+  </si>
+  <si>
+    <t>New Dataset</t>
+  </si>
+  <si>
+    <t>..\..\..\..\..\documents\Book1.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nothing</t>
+  </si>
+  <si>
+    <t>Duval</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Duval.m</t>
+  </si>
+  <si>
+    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
+2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
+  </si>
+  <si>
+    <t>Rogers' 4</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Roger4.m</t>
+  </si>
+  <si>
+    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
+ 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>IEC 60599</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_IEC.m</t>
+  </si>
+  <si>
+    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>Clustering (Fortran)</t>
+  </si>
+  <si>
+    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
+  </si>
+  <si>
+    <t>Cond. prob.</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Cond_Prob.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_ANN.m</t>
+  </si>
+  <si>
+    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
+  </si>
+  <si>
+    <t>IEC 60599 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\IEC_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
+  </si>
+  <si>
+    <t>Rogers' 4 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\ROG_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t>Duval (C++)</t>
+  </si>
+  <si>
+    <t>.\methods\cpp\release\DGA_Test.exe</t>
+  </si>
+  <si>
+    <t>To demonstrate the integration of DAG method implementation in C++ language</t>
   </si>
 </sst>
 </file>
@@ -1142,16 +1151,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="91.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="91.44140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1168,116 +1177,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60">
+    <row r="2" spans="1:4" ht="57.6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="165">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="158.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="165">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="158.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2">
       <c r="A5" s="3">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2">
       <c r="A6" s="3">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="135">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="129.6">
       <c r="A7" s="3">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2">
       <c r="A8" s="3">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2">
       <c r="A9" s="3">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1285,13 +1294,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1302,16 +1311,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="76" style="2" customWidth="1"/>
   </cols>
@@ -1330,172 +1339,186 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="28.8">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="255">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="244.8">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="180">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="144">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1533,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code reorganization and bug fixes
* Combined DGA_1, DGA_n into DGAs_n script.
* Fixed missing ‘\’ at the end of relative path in some cases.
* Improved the exported graph format
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="432" windowWidth="24492" windowHeight="15972"/>
+    <workbookView xWindow="0" yWindow="432" windowWidth="24492" windowHeight="15972" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,93 @@
     <t>ID</t>
   </si>
   <si>
+    <t>Duval</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Duval.m</t>
+  </si>
+  <si>
+    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
+2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
+  </si>
+  <si>
+    <t>Rogers' 4</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Roger4.m</t>
+  </si>
+  <si>
+    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
+ 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>IEC 60599</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_IEC.m</t>
+  </si>
+  <si>
+    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
+2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
+  </si>
+  <si>
+    <t>Clustering (Fortran)</t>
+  </si>
+  <si>
+    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
+  </si>
+  <si>
+    <t>Cond. prob.</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_Cond_Prob.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>.\methods\DGA_ANN.m</t>
+  </si>
+  <si>
+    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
+2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
+3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
+  </si>
+  <si>
+    <t>IEC 60599 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\IEC_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
+  </si>
+  <si>
+    <t>Rogers' 4 Refined</t>
+  </si>
+  <si>
+    <t>.\methods\ROG_REFINNING_NEW.m</t>
+  </si>
+  <si>
+    <t>Duval (C++)</t>
+  </si>
+  <si>
+    <t>.\methods\cpp\release\DGA_Test.exe</t>
+  </si>
+  <si>
+    <t>To demonstrate the integration of DAG method implementation in C++ language</t>
+  </si>
+  <si>
     <t>Lab Data (240)</t>
   </si>
   <si>
@@ -152,100 +239,13 @@
 3. O.E Gouda, Saber Salem and Salah Hamdy El-Hoshy “Power transformer incipient faults diagnosis based on dissolved gas analysis”, TELKOMNIKA Indonesian Journal of Electrical Engineering Vol. 17, No. 1, pp. 10 ~ 16,  January 2016.</t>
   </si>
   <si>
-    <t>New Dataset</t>
-  </si>
-  <si>
-    <t>..\..\..\..\..\documents\Book1.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nothing</t>
-  </si>
-  <si>
-    <t>Duval</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Duval.m</t>
-  </si>
-  <si>
-    <t>1. Duval, M.: "A review of faults detectable by gas-in-oil analysis in transformers", IEEE Electr. Insul. Mag., 18, (3), pp. 8–17, 2002.
-2. Duval, M.: "Interpretation of gas-in-oil analysis using new IEC publication 60599 and IEC TC 10 databases", IEEE Electr. Insul. Mag., 17, (2), pp. 31–41, 2001.</t>
-  </si>
-  <si>
-    <t>Rogers' 4</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Roger4.m</t>
-  </si>
-  <si>
-    <t>1. IEEE Guide for the Interpretation of Gases Generated in Oil-Immersed Transformers, IEEE Standard C57.104-2008, Feb. 2009.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016.
- 3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>IEC 60599</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_IEC.m</t>
-  </si>
-  <si>
-    <t>1. IEC Publication 599, “Interpretation of the analysis of gases in transformers and other oil-filled electrical equipment in service,” First Edition 1978.
-2. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-3. J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-4. Ibrahim B. M. Taha, Sherif S. M. Ghoneim, and Hatim G. Zaini, "A Fuzzy Diagnostic System for Incipient Transformer Faults Based on DGA of the Insulating Transformer Oils", International Review of Electrical Engineering (I.R.E.E.), Vol. 11, n. 3, pp. 305-313, June 2016.</t>
-  </si>
-  <si>
-    <t>Clustering (Fortran)</t>
-  </si>
-  <si>
-    <t>.\methods\fortran\build\DGA_Clustering.exe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sherif S. M. Ghoneim, and Ibrahim B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
-  </si>
-  <si>
-    <t>Cond. prob.</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_Cond_Prob.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, Diaa A. Mansour, Sherif S. M. Ghoneim, Nagy I. Elkalashy," Conditional Probability-Based Interpretation of Dissolved Gas Analysis for Transformer Incipient Faults", IET Generation, Transmission &amp; Distribution, Vol. 11, No. 4, pp. 943 – 951, 2017.</t>
-  </si>
-  <si>
-    <t>ANN</t>
-  </si>
-  <si>
-    <t>.\methods\DGA_ANN.m</t>
-  </si>
-  <si>
-    <t>1. Sherif S. M. Ghoneim, and I. B. M. Taha, and N. I. Elkalashy," Integrated ANN-Based Proactive Fault Diagnostic Scheme for Power Transformers Using Dissolved Gas Analysis", IEEE Transactions on Dielectric and Electrical Insulation, Vol. 23, No. 3, pp. 1838-1845, June 2016. 
-2.  J. L. Guardado, J. L. Nared, P. Moreno, and C. R. Fuerte, "A Comparative Study of Neural Network Efficiency in Power Transformers Diagnosis Using Dissolved Gas Analysis", IEEE Trans. Power Delivery, Vol. 16, No. 4, pp. 643 – 647, 2001.
-3.  V. Miranda, A. R. Garez Castro, and Sh. Lima, "Diagnosing Faults in Power Transformers with Autoassociative Neural Networks and Mean Shift", IEEE Trans. Power Delivery, Vol. 27, No. 3, pp. 1350 – 1357, 2012.</t>
-  </si>
-  <si>
-    <t>IEC 60599 Refined</t>
-  </si>
-  <si>
-    <t>.\methods\IEC_REFINNING_NEW.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ibrahim B. M. Taha, and Sherif S. M. Ghoneim, and Abdulaziz. S. A. Duaywah, " Refining DGA Methods of IEC Code and Rogers Four Ratios for Transformer Fault Diagnosis", 2016 IEEE PES General Meeting, Boston, USA, 17-21 July 2016.</t>
-  </si>
-  <si>
-    <t>Rogers' 4 Refined</t>
-  </si>
-  <si>
-    <t>.\methods\ROG_REFINNING_NEW.m</t>
-  </si>
-  <si>
-    <t>Duval (C++)</t>
-  </si>
-  <si>
-    <t>.\methods\cpp\release\DGA_Test.exe</t>
-  </si>
-  <si>
-    <t>To demonstrate the integration of DAG method implementation in C++ language</t>
+    <t xml:space="preserve">Diagnosis </t>
+  </si>
+  <si>
+    <t>.\datasets\diagnosis_only.xlsx</t>
+  </si>
+  <si>
+    <t>A sample to test diagnosis without having an "actual" diagnosis column available.</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
@@ -1182,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="158.4">
@@ -1196,13 +1196,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="158.4">
@@ -1210,13 +1210,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.2">
@@ -1224,13 +1224,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2">
@@ -1238,13 +1238,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="129.6">
@@ -1252,13 +1252,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2">
@@ -1266,13 +1266,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2">
@@ -1280,13 +1280,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1294,13 +1294,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
@@ -1344,13 +1344,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8">
@@ -1358,13 +1358,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8">
@@ -1372,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.2">
@@ -1386,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2">
@@ -1400,13 +1400,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8">
@@ -1414,13 +1414,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2">
@@ -1428,13 +1428,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="244.8">
@@ -1442,13 +1442,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.2">
@@ -1456,13 +1456,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2">
@@ -1470,13 +1470,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57.6">
@@ -1484,13 +1484,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="144">
@@ -1498,13 +1498,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1512,13 +1512,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validation dataset, gui formatting
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saleh\Documents\GitHub\DGA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AC3C14-26FE-4472-804B-802CC36F75F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="432" windowWidth="24492" windowHeight="15972" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="24495" windowHeight="15975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Filename</t>
   </si>
@@ -247,11 +253,20 @@
   <si>
     <t>A sample to test diagnosis without having an "actual" diagnosis column available.</t>
   </si>
+  <si>
+    <t>Clustering Test</t>
+  </si>
+  <si>
+    <t>.\datasets\test_clustering.xlsx</t>
+  </si>
+  <si>
+    <t>S. S. M. Ghoneim, and I. B. M. Taha,"A New Approach of DGA Interpretation Technique for Transformer Fault Diagnosis", International Journal of Electrical Power and Energy Systems, 81, Oct. 2016, pp. 265–274.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -803,51 +818,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
-    <cellStyle name="20% - Accent1 2" xfId="5"/>
-    <cellStyle name="20% - Accent2 2" xfId="6"/>
-    <cellStyle name="20% - Accent3 2" xfId="7"/>
-    <cellStyle name="20% - Accent4 2" xfId="8"/>
-    <cellStyle name="20% - Accent5 2" xfId="9"/>
-    <cellStyle name="20% - Accent6 2" xfId="10"/>
-    <cellStyle name="40% - Accent1 2" xfId="11"/>
-    <cellStyle name="40% - Accent2 2" xfId="12"/>
-    <cellStyle name="40% - Accent3 2" xfId="13"/>
-    <cellStyle name="40% - Accent4 2" xfId="14"/>
-    <cellStyle name="40% - Accent5 2" xfId="15"/>
-    <cellStyle name="40% - Accent6 2" xfId="16"/>
-    <cellStyle name="60% - Accent1 2" xfId="17"/>
-    <cellStyle name="60% - Accent2 2" xfId="18"/>
-    <cellStyle name="60% - Accent3 2" xfId="19"/>
-    <cellStyle name="60% - Accent4 2" xfId="20"/>
-    <cellStyle name="60% - Accent5 2" xfId="21"/>
-    <cellStyle name="60% - Accent6 2" xfId="22"/>
-    <cellStyle name="Accent1 2" xfId="23"/>
-    <cellStyle name="Accent2 2" xfId="24"/>
-    <cellStyle name="Accent3 2" xfId="25"/>
-    <cellStyle name="Accent4 2" xfId="26"/>
-    <cellStyle name="Accent5 2" xfId="27"/>
-    <cellStyle name="Accent6 2" xfId="28"/>
-    <cellStyle name="Bad 2" xfId="29"/>
-    <cellStyle name="Calculation 2" xfId="30"/>
-    <cellStyle name="Check Cell 2" xfId="31"/>
-    <cellStyle name="Explanatory Text 2" xfId="32"/>
+    <cellStyle name="20% - Accent1 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Calculation 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Check Cell 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Good 2" xfId="33"/>
-    <cellStyle name="Heading 1 2" xfId="34"/>
-    <cellStyle name="Heading 2 2" xfId="35"/>
-    <cellStyle name="Heading 3 2" xfId="36"/>
-    <cellStyle name="Heading 4 2" xfId="37"/>
+    <cellStyle name="Good 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Heading 1 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Heading 2 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Heading 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Heading 4 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Input 2" xfId="38"/>
-    <cellStyle name="Linked Cell 2" xfId="39"/>
-    <cellStyle name="Neutral 2" xfId="40"/>
+    <cellStyle name="Input 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Neutral 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="Note" xfId="3" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="41"/>
-    <cellStyle name="Title 2" xfId="42"/>
-    <cellStyle name="Total 2" xfId="43"/>
-    <cellStyle name="Warning Text 2" xfId="44"/>
+    <cellStyle name="Output 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Title 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Total 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Warning Text 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1148,19 +1163,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="91.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="91.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1177,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57.6">
+    <row r="2" spans="1:4" ht="60">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1191,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="158.4">
+    <row r="3" spans="1:4" ht="165">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1205,7 +1220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="158.4">
+    <row r="4" spans="1:4" ht="165">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1219,7 +1234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2">
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1233,7 +1248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1247,7 +1262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="129.6">
+    <row r="7" spans="1:4" ht="135">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1261,7 +1276,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.2">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1275,7 +1290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.2">
+    <row r="9" spans="1:4" ht="45">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1310,17 +1325,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="76" style="2" customWidth="1"/>
   </cols>
@@ -1339,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1381,7 +1396,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2">
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1395,7 +1410,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.2">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1437,7 +1452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="244.8">
+    <row r="9" spans="1:4" ht="255">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1451,7 +1466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.2">
+    <row r="10" spans="1:4" ht="60">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.2">
+    <row r="11" spans="1:4" ht="45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="57.6">
+    <row r="12" spans="1:4" ht="60">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1493,7 +1508,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="144">
+    <row r="13" spans="1:4" ht="180">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1519,6 +1534,20 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1528,12 +1557,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>